<commit_message>
feat(questions): modify import with new template excel, add export questions via excel, docx, txt
</commit_message>
<xml_diff>
--- a/templates/excels/TemplateImportQuestions.xlsx
+++ b/templates/excels/TemplateImportQuestions.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,24 +409,29 @@
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="15.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="20.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="12.83203125" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" customWidth="1"/>
+    <col min="24" max="24" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>TEMPLATE IMPORT QUESTIONS</v>
+        <v>Import Questions Via Excel</v>
       </c>
       <c r="B1" t="str">
         <v/>
@@ -480,6 +485,21 @@
         <v/>
       </c>
       <c r="S1" t="str">
+        <v/>
+      </c>
+      <c r="T1" t="str">
+        <v/>
+      </c>
+      <c r="U1" t="str">
+        <v/>
+      </c>
+      <c r="V1" t="str">
+        <v/>
+      </c>
+      <c r="W1" t="str">
+        <v/>
+      </c>
+      <c r="X1" t="str">
         <v/>
       </c>
     </row>
@@ -503,102 +523,132 @@
         <v>A</v>
       </c>
       <c r="G2" t="str">
+        <v>A_correct</v>
+      </c>
+      <c r="H2" t="str">
         <v>B</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
+        <v>B_correct</v>
+      </c>
+      <c r="J2" t="str">
         <v>C</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
+        <v>C_correct</v>
+      </c>
+      <c r="L2" t="str">
         <v>D</v>
       </c>
-      <c r="J2" t="str">
+      <c r="M2" t="str">
+        <v>D_correct</v>
+      </c>
+      <c r="N2" t="str">
         <v>E</v>
       </c>
-      <c r="K2" t="str">
+      <c r="O2" t="str">
+        <v>E_correct</v>
+      </c>
+      <c r="P2" t="str">
         <v>F</v>
       </c>
-      <c r="L2" t="str">
+      <c r="Q2" t="str">
+        <v>F_correct</v>
+      </c>
+      <c r="R2" t="str">
         <v>G</v>
       </c>
-      <c r="M2" t="str">
+      <c r="S2" t="str">
+        <v>G_correct</v>
+      </c>
+      <c r="T2" t="str">
         <v>H</v>
       </c>
-      <c r="N2" t="str">
-        <v>I</v>
-      </c>
-      <c r="O2" t="str">
-        <v>J</v>
-      </c>
-      <c r="P2" t="str">
-        <v>correct_answers</v>
-      </c>
-      <c r="Q2" t="str">
+      <c r="U2" t="str">
+        <v>H_correct</v>
+      </c>
+      <c r="V2" t="str">
         <v>is_public</v>
       </c>
-      <c r="R2" t="str">
+      <c r="W2" t="str">
         <v>options_json</v>
       </c>
-      <c r="S2" t="str">
+      <c r="X2" t="str">
         <v>status</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Nội dung câu hỏi (required)</v>
+        <v>Question content (required)</v>
       </c>
       <c r="B3" t="str">
-        <v>multiple_choice/essay (required)</v>
+        <v>multiple_choice or essay (required)</v>
       </c>
       <c r="C3" t="str">
-        <v>Tên danh mục (optional)</v>
+        <v>Category name (optional, auto-create if new)</v>
       </c>
       <c r="D3" t="str">
-        <v>easy/medium/hard (optional)</v>
+        <v>easy, medium, or hard (optional, default: medium)</v>
       </c>
       <c r="E3" t="str">
-        <v>true/false (optional)</v>
+        <v>TRUE or FALSE (optional, default: FALSE)</v>
       </c>
       <c r="F3" t="str">
-        <v>Đáp án A</v>
+        <v>Option A text</v>
       </c>
       <c r="G3" t="str">
-        <v>Đáp án B</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="H3" t="str">
-        <v>Đáp án C</v>
+        <v>Option B text</v>
       </c>
       <c r="I3" t="str">
-        <v>Đáp án D</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="J3" t="str">
-        <v>Đáp án E</v>
+        <v>Option C text</v>
       </c>
       <c r="K3" t="str">
-        <v>Đáp án F</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="L3" t="str">
-        <v>Đáp án G</v>
+        <v>Option D text</v>
       </c>
       <c r="M3" t="str">
-        <v>Đáp án H</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="N3" t="str">
-        <v>Đáp án I</v>
+        <v>Option E text</v>
       </c>
       <c r="O3" t="str">
-        <v>Đáp án J</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="P3" t="str">
-        <v>Đáp án đúng (vd: 1,2,3) (required for multiple_choice)</v>
+        <v>Option F text</v>
       </c>
       <c r="Q3" t="str">
-        <v>true/false (optional)</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
       </c>
       <c r="R3" t="str">
-        <v>Bỏ qua</v>
+        <v>Option G text</v>
       </c>
       <c r="S3" t="str">
-        <v>Kiểm lỗi (auto)</v>
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
+      </c>
+      <c r="T3" t="str">
+        <v>Option H text</v>
+      </c>
+      <c r="U3" t="str">
+        <v>TRUE or FALSE (leave empty = FALSE)</v>
+      </c>
+      <c r="V3" t="str">
+        <v>TRUE or FALSE (optional)</v>
+      </c>
+      <c r="W3" t="str">
+        <v>Auto-filled, ignore</v>
+      </c>
+      <c r="X3" t="str">
+        <v>Error messages (auto-filled)</v>
       </c>
     </row>
     <row r="4">
@@ -614,32 +664,32 @@
       <c r="D4" t="str">
         <v>easy</v>
       </c>
-      <c r="E4" t="str">
-        <v>false</v>
+      <c r="E4" t="b">
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <v>YES</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
         <v>NO</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="str">
         <v>MAYBE</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="str">
         <v>ALL</v>
       </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
+      <c r="M4" t="b">
+        <v>0</v>
       </c>
       <c r="N4" t="str">
         <v/>
@@ -648,15 +698,30 @@
         <v/>
       </c>
       <c r="P4" t="str">
-        <v>2</v>
+        <v/>
       </c>
       <c r="Q4" t="str">
-        <v>false</v>
+        <v/>
       </c>
       <c r="R4" t="str">
         <v/>
       </c>
       <c r="S4" t="str">
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <v/>
+      </c>
+      <c r="U4" t="str">
+        <v/>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="str">
+        <v/>
+      </c>
+      <c r="X4" t="str">
         <v/>
       </c>
     </row>
@@ -673,49 +738,64 @@
       <c r="D5" t="str">
         <v>medium</v>
       </c>
-      <c r="E5" t="str">
-        <v>true</v>
+      <c r="E5" t="b">
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <v>Python</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
         <v>HTML</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
         <v>JavaScript</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="str">
         <v>CSS</v>
       </c>
-      <c r="J5" t="str">
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="str">
         <v>Java</v>
       </c>
-      <c r="K5" t="str">
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="str">
         <v>SQL</v>
       </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
-        <v/>
-      </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-      <c r="P5" t="str">
-        <v>1,3,5</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>true</v>
+      <c r="Q5" t="b">
+        <v>0</v>
       </c>
       <c r="R5" t="str">
         <v/>
       </c>
       <c r="S5" t="str">
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <v/>
+      </c>
+      <c r="U5" t="str">
+        <v/>
+      </c>
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="str">
+        <v/>
+      </c>
+      <c r="X5" t="str">
         <v/>
       </c>
     </row>
@@ -732,8 +812,8 @@
       <c r="D6" t="str">
         <v>hard</v>
       </c>
-      <c r="E6" t="str">
-        <v>false</v>
+      <c r="E6" t="b">
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <v/>
@@ -769,18 +849,33 @@
         <v/>
       </c>
       <c r="Q6" t="str">
-        <v>false</v>
+        <v/>
       </c>
       <c r="R6" t="str">
         <v/>
       </c>
       <c r="S6" t="str">
+        <v/>
+      </c>
+      <c r="T6" t="str">
+        <v/>
+      </c>
+      <c r="U6" t="str">
+        <v/>
+      </c>
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" t="str">
+        <v/>
+      </c>
+      <c r="X6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -799,13 +894,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>TYPE</v>
+        <v>type</v>
       </c>
       <c r="B1" t="str">
-        <v>DIFFICULTY</v>
+        <v>difficulty</v>
       </c>
       <c r="C1" t="str">
-        <v>BOOLEAN</v>
+        <v>boolean</v>
       </c>
     </row>
     <row r="2">
@@ -815,8 +910,8 @@
       <c r="B2" t="str">
         <v>easy</v>
       </c>
-      <c r="C2" t="str">
-        <v>true</v>
+      <c r="C2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -826,8 +921,8 @@
       <c r="B3" t="str">
         <v>medium</v>
       </c>
-      <c r="C3" t="str">
-        <v>false</v>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>